<commit_message>
a new commit message for Excel test from github API
</commit_message>
<xml_diff>
--- a/TestGit.xlsx
+++ b/TestGit.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mydrive.gsk.com/personal/santhanathan_x_k_gsk_com/Documents/Documents/stories/GitHub_Discovery/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sk511017\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="11_F25DC773A252ABDACC10481CF1DC471C5BDE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6E0F4AF1-18DA-49E7-9EBB-559BDE9D7ACE}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73DABBB5-7A44-4584-A9F3-BD997CEC3413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Apple</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>Mango</t>
+  </si>
+  <si>
+    <t>Sell value actual</t>
   </si>
 </sst>
 </file>
@@ -360,15 +363,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -378,8 +384,11 @@
       <c r="C1" t="s">
         <v>3</v>
       </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -389,8 +398,11 @@
       <c r="C2">
         <v>20</v>
       </c>
+      <c r="D2">
+        <v>15</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -400,8 +412,11 @@
       <c r="C3">
         <v>10</v>
       </c>
+      <c r="D3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -410,6 +425,9 @@
       </c>
       <c r="C4">
         <v>30</v>
+      </c>
+      <c r="D4">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>